<commit_message>
[transaction] Added apis for transaction service impl: controller, service, repo
</commit_message>
<xml_diff>
--- a/data/excel/Book1.xlsx
+++ b/data/excel/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\com\AppData\Roaming\Microsoft\Windows\Network Shortcuts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jikku\Study\Jikks Studies\workspace\abc-mortgage-banking\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45006BD-B57B-43F7-AED7-8672E23A95CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E97263-5CE6-4958-96A7-89FA6E64F20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6BA37BFF-D60A-4AD5-8683-7943F8452078}"/>
+    <workbookView minimized="1" xWindow="5640" yWindow="3780" windowWidth="16920" windowHeight="10540" activeTab="1" xr2:uid="{6BA37BFF-D60A-4AD5-8683-7943F8452078}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -346,9 +346,6 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -361,6 +358,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -380,9 +380,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -420,7 +420,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -526,7 +526,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -668,7 +668,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -678,59 +678,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2296E044-DDF7-4ECD-87A1-CD4DE55981D6}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="2" max="2" width="25.1796875" hidden="1" customWidth="1"/>
+    <col min="3" max="4" width="25.1796875" customWidth="1"/>
     <col min="5" max="5" width="35.90625" customWidth="1"/>
-    <col min="6" max="6" width="35.90625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="35.90625" style="2" customWidth="1"/>
     <col min="7" max="7" width="17.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="2"/>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C3" t="s">
@@ -742,7 +744,7 @@
       <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G3" t="s">
@@ -759,7 +761,7 @@
       <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G4" t="s">
@@ -776,7 +778,7 @@
       <c r="E5" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G5" t="s">
@@ -790,10 +792,10 @@
       <c r="D6" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G6" t="s">
@@ -810,7 +812,7 @@
       <c r="E7" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G7" t="s">
@@ -827,7 +829,7 @@
       <c r="E8" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>35</v>
       </c>
       <c r="G8" t="s">
@@ -850,7 +852,7 @@
       <c r="E10" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G10" t="s">
@@ -864,10 +866,10 @@
       <c r="D11" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>44</v>
       </c>
       <c r="G11" t="s">
@@ -881,10 +883,10 @@
       <c r="D12" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>45</v>
       </c>
       <c r="G12" t="s">
@@ -898,10 +900,10 @@
       <c r="D13" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>46</v>
       </c>
       <c r="G13" t="s">
@@ -918,10 +920,10 @@
       <c r="D16" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>47</v>
       </c>
       <c r="G16" t="s">
@@ -935,10 +937,10 @@
       <c r="D17" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G17" t="s">
@@ -955,10 +957,10 @@
       <c r="D19" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>54</v>
       </c>
       <c r="G19" t="s">
@@ -972,10 +974,10 @@
       <c r="D20" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>55</v>
       </c>
       <c r="G20" t="s">
@@ -994,7 +996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8FE7DC0-76C0-4E60-90B2-0737E41AC382}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1009,19 +1011,19 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:2" ht="243" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:2" ht="173.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1029,7 +1031,7 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1037,7 +1039,7 @@
       <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>